<commit_message>
Mis à jour du suivi
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan\Documents\Git\LaboSystemNumeric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hearc365-my.sharepoint.com/personal/gabriel_dostuni_he-arc_ch/Documents/Documents/HeArc/ISC1b/systemes_numériques/LaboSystemNumeric/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FA405F-DD1E-4DA6-8758-6D32D135B45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{B5FA405F-DD1E-4DA6-8758-6D32D135B45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA79B6A8-0639-411E-A9F3-7EB95FDA9903}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travail" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Durée</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>Programmation de la rom</t>
+  </si>
+  <si>
+    <t>2h00</t>
+  </si>
+  <si>
+    <t>Programmation de la rom et création du test bench</t>
+  </si>
+  <si>
+    <t>Debug du code grâce à la carte et correction de certain bug</t>
   </si>
 </sst>
 </file>
@@ -461,7 +470,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,24 +672,48 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
+      <c r="B10" s="7">
+        <v>45384</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="7">
+        <v>45384</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="7">
+        <v>45391</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
+      <c r="F11" s="7">
+        <v>45391</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
created the Rendu 4
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hearc365-my.sharepoint.com/personal/gabriel_dostuni_he-arc_ch/Documents/Documents/HeArc/ISC1b/systemes_numériques/LaboSystemNumeric/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan\Documents\Git\LaboSystemNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{57883AFF-CD27-494F-9C2B-6635A228F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38D0212C-8A4A-43B6-A396-17B11C658D26}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A4D4A4-2A87-46DD-9431-C6361CDE32BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travail" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Durée</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Modifier le nanoProcesseur / nanoControlleur pour ajouter les appels d'interruptions</t>
+  </si>
+  <si>
+    <t>25m</t>
+  </si>
+  <si>
+    <t>modifications dans le graph d'état</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,13 +776,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="7">
+        <v>45412</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="7">
+        <v>45412</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tried to fix the sequencer
</commit_message>
<xml_diff>
--- a/Suivi.xlsx
+++ b/Suivi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabdo\OneDrive - HE-ARC\Documents\HeArc\ISC1b\systemes_numériques\LaboSystemNumeric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stan\Documents\Git\LaboSystemNumeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CFBD34-4F4C-4421-A9B0-94036C22A50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CDDBA8-8E73-4DC8-B94A-0C1B5894AE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Travail" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Durée</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Continuation du test bench</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>Essai pour faire fonctionner le séquenceur</t>
+  </si>
+  <si>
+    <t>Continuation de testbench et des corrections</t>
   </si>
 </sst>
 </file>
@@ -497,7 +506,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,24 +915,48 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
+      <c r="B19" s="7">
+        <v>45451</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
+      <c r="F19" s="7">
+        <v>45451</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
+      <c r="B20" s="7">
+        <v>45453</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="3"/>
+      <c r="F20" s="7">
+        <v>45453</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>